<commit_message>
Update logboek & Technical and functional analysis - Accelerometer Thread - Matter V02.docx
</commit_message>
<xml_diff>
--- a/Logboek/LOGBOEK.xlsx
+++ b/Logboek/LOGBOEK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bart\School\WERKPLEKLEREN\Project Thread Matter\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D446750A-FE47-48AA-AB6A-26AB09CC3627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A96DB5-530D-4930-B94E-74B00A1DE21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="1395" windowWidth="21600" windowHeight="11505" xr2:uid="{316E3ABB-5740-4A1B-97C2-BFA25A54D4CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{316E3ABB-5740-4A1B-97C2-BFA25A54D4CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Brainstorm voor het project, start technische analyse en component keuze</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Verder gewerkt met het bare-metal project. UART nog verder getest. Gyroscope uitgezocht en getest, ook accelerometer uitgezocht en getest. Beslissing genomen om verder te gaan met de acceleromtere ipv gyroscope omdat deze zijn value behoudt, dan kan de value (positie van de controller) worden toegewezen aan een positie in de game.</t>
+  </si>
+  <si>
+    <t>Testen dat ik heb uitgevoerd gedocumenteerd. Verdere documentatie over het Matter protocol</t>
+  </si>
+  <si>
+    <t>De testen level-control en accelerometer willen combineren in één project. Tussentijds een update van de SDK gedaan. Bij het debuggen kreeg ik de volgende error: WARNING: Failed to read memory @ address 0xFFFFFFFE. Ik kreeg dit niet opgelost.</t>
+  </si>
+  <si>
+    <t>IDE opnieuw geinstalleerd om probleem te verhelpen maar is niet gelukt.</t>
+  </si>
+  <si>
+    <t>Verder gewerkt aan technische analyse sectie Matter Interaction model. Probleem van de mcu is opgelost, er was een probleem met de bootloader. De oplossing was door een project te gebruiken met een external bootloader, eerst de bootloader geflashed en daarna de firmware. Nu werkt het terug.</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -141,6 +153,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,18 +520,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9F47F0-0464-45B2-8090-3D59A1696249}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="112.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="112.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -527,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -538,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -549,7 +564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -560,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -571,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -582,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -593,7 +608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -604,7 +619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -615,7 +630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -626,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -637,7 +652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -648,7 +663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -659,7 +674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -670,7 +685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -681,43 +696,51 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="3">
         <v>45281</v>
       </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>44944</v>
       </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="3">
         <v>44951</v>
       </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="3">
         <v>44958</v>
       </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -726,7 +749,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -735,7 +758,7 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -744,7 +767,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -753,7 +776,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -762,7 +785,7 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -771,7 +794,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -780,7 +803,7 @@
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -789,7 +812,7 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -798,7 +821,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -807,7 +830,7 @@
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -816,45 +839,45 @@
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logboek updated Technische Analyse updated
</commit_message>
<xml_diff>
--- a/Logboek/LOGBOEK.xlsx
+++ b/Logboek/LOGBOEK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bart\School\WERKPLEKLEREN\Project Thread Matter\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A96DB5-530D-4930-B94E-74B00A1DE21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC36E45A-209B-413D-8D40-D1607AE5C032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{316E3ABB-5740-4A1B-97C2-BFA25A54D4CC}"/>
+    <workbookView xWindow="3225" yWindow="1890" windowWidth="21600" windowHeight="11430" xr2:uid="{316E3ABB-5740-4A1B-97C2-BFA25A54D4CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Brainstorm voor het project, start technische analyse en component keuze</t>
   </si>
@@ -87,10 +87,22 @@
     <t>De testen level-control en accelerometer willen combineren in één project. Tussentijds een update van de SDK gedaan. Bij het debuggen kreeg ik de volgende error: WARNING: Failed to read memory @ address 0xFFFFFFFE. Ik kreeg dit niet opgelost.</t>
   </si>
   <si>
-    <t>IDE opnieuw geinstalleerd om probleem te verhelpen maar is niet gelukt.</t>
-  </si>
-  <si>
-    <t>Verder gewerkt aan technische analyse sectie Matter Interaction model. Probleem van de mcu is opgelost, er was een probleem met de bootloader. De oplossing was door een project te gebruiken met een external bootloader, eerst de bootloader geflashed en daarna de firmware. Nu werkt het terug.</t>
+    <t>Verder gewerkt aan technische analyse sectie Matter Interaction model. Probleem van de mcu is opgelost, er was een probleem met de bootloader. De oplossing was door een project te gebruiken met een external bootloader, eerst de bootloader geflashed en daarna de applicatie. Nu werkt het terug. De applicatie die ik heb gebruikt was een example project, "MatterSensorOverThread" in simplicity studio. Hier heb ik momenteel nog niets in aangepast.</t>
+  </si>
+  <si>
+    <t>IDE opnieuw geinstalleerd om probleem te verhelpen maar is niet gelukt. Voor de rest nog veel dingen geprobeerd om alles aan de praat te krijgen maar niets hielp.</t>
+  </si>
+  <si>
+    <t>Nieuw project aangemaakt met bootloader "MatterAccelerometerThread". In dit project ga ik alles aanpassen zodat ik mijn sensor kan uitlezen. Hier terug gestart van hetzelfde example project. De file SensorCallback.cpp verwijderd en een nieuwe aangemaakt "SensorManager.cpp" in deze file ga ik alle fucnties maken die relevant zijn voor de sensor. Compileren werkt maar de sensor krijgt geen data, nog verder uit te zoeken.</t>
+  </si>
+  <si>
+    <t>Probleem uitgezocht met de sensor, logic analyzer aan het bordje gehangen op de SPI lines en hier zag ik dat de MOSI constant hoog was en niet veranderden bij het transmitten. Voor te controlleren welke SPI modi nodig zijn voor de sensor heb ik een bare-metal project gemaakt met de sensor om zo de lijnen uit te lezen. Hieruit bleek dat zowel MOSI als MISO en CLOCK idle laag zijn. Hieruit wist ik dus dat er ergens een probleem was in de configuratie van de SPI. Verder in de code gaan zoeken maar had nergens iets gevonden. Uiteindelijk er achter gekomen dat de bootloader met een externe flash kan werken, in de datasheet gekeken en de externe flash wordt gebruikt via SPI. Dan ben ik in de configuratie van de bootloader gaan kijken en daar heb ik dan gevonden dat de bootloader de SPI blokkeert. Dit heb ik af gezet en dan werkte alles. Verder heb ik gezocht naar een breakout game in Python, ik heb twee games gevonden en in de code gezocht naar hoe ik dit kon manipuleren.</t>
+  </si>
+  <si>
+    <t>Een keuze gemaakt welke Python game ik ga gebruiken. Onderzocht hoe ik nu het beste de data kan uitlezen, gewoon data opvragen met de CHIP-Tool is niet snel genoeg. De oplossing is door het interactieve proces van de CHIP-Tool te kunnen gebruiken. Code aangepast zodat de game bestuurbaar wordt via Matter over Thread. Dit heb ik gedaan door vanuit de game een nieuwe thread te starten zodat het lezen van de sensor de snelheid van de game niet beinvloed. In de thread gaan we de nodige commando's sturen zodat het interactive process gestart kan worden, dan wordt alles gefilterd zodat we enkel de data van de sensor overhouden. Dit wordt dan gebruikt om de paddle te bedienen.</t>
+  </si>
+  <si>
+    <t>Gewerkt aan de documentatie.</t>
   </si>
 </sst>
 </file>
@@ -141,21 +153,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9F47F0-0464-45B2-8090-3D59A1696249}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,301 +560,311 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>45183</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>45190</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>45197</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>45204</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>45211</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>45218</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>45225</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>45232</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>45239</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>45246</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>45253</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>45261</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>45267</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>45275</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="5">
         <v>45281</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="5">
         <v>44944</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>44951</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <v>44958</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3">
-        <v>44958</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>44965</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <v>44972</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5">
+        <v>44979</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3">
-        <v>44965</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3">
-        <v>44972</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3">
-        <v>44979</v>
-      </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>21</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="5">
         <v>44992</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="5">
         <v>44999</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="5">
         <v>45006</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="5">
         <v>45013</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="5">
         <v>45034</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="5">
         <v>45041</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="5">
         <v>45048</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>

</xml_diff>